<commit_message>
do n2o start fuel
</commit_message>
<xml_diff>
--- a/R/data_raw/lca-sheets/enterprise-flows-all-areas.xlsx
+++ b/R/data_raw/lca-sheets/enterprise-flows-all-areas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\alfalfa\R\data_raw\lca-sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C699FC59-6C0F-4071-BEE6-E42D7B73024D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806B6B27-6E7B-4A00-AEE1-A72AC588716B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{6B1DF06E-0D8B-4B6A-BB9B-61BA1D32BA21}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="8" xr2:uid="{6B1DF06E-0D8B-4B6A-BB9B-61BA1D32BA21}"/>
   </bookViews>
   <sheets>
     <sheet name="meta-data" sheetId="10" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="106">
   <si>
     <t>units</t>
   </si>
@@ -131,9 +131,6 @@
     <t>the timeline visual was used to create this table (in docs folder)</t>
   </si>
   <si>
-    <t>disc</t>
-  </si>
-  <si>
     <t>note the seed could be round-up ready or not, may impact embodied energy</t>
   </si>
   <si>
@@ -203,9 +200,6 @@
     <t>From San Joaquin organic enterprise budget, which includes rough estimates for inter-mountain, valleys, and imperial valleys - this one represents the sacramento/san joaquin valley</t>
   </si>
   <si>
-    <t>organic, central valley</t>
-  </si>
-  <si>
     <t>4 year stand life</t>
   </si>
   <si>
@@ -230,9 +224,6 @@
     <t>Ash or limestone</t>
   </si>
   <si>
-    <t>tualre county</t>
-  </si>
-  <si>
     <t>If there is insufficient rain in the fall/winter of establishment two irrigations of 8 ac-in may be needed, otherwise only one</t>
   </si>
   <si>
@@ -329,9 +320,6 @@
     <t>roll</t>
   </si>
   <si>
-    <t>disc border ridges</t>
-  </si>
-  <si>
     <t>fertilize</t>
   </si>
   <si>
@@ -354,6 +342,27 @@
   </si>
   <si>
     <t>round-up ready seed</t>
+  </si>
+  <si>
+    <t>tulare_county</t>
+  </si>
+  <si>
+    <t>central_valley_organic</t>
+  </si>
+  <si>
+    <t>tualre_county</t>
+  </si>
+  <si>
+    <t>stand_life_yrs</t>
+  </si>
+  <si>
+    <t>mid, best, and worst are the same right now</t>
+  </si>
+  <si>
+    <t>disk</t>
+  </si>
+  <si>
+    <t>disk border ridges</t>
   </si>
 </sst>
 </file>
@@ -744,7 +753,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -755,7 +764,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -767,43 +776,43 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -811,7 +820,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
@@ -819,7 +828,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -827,7 +836,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -864,7 +873,7 @@
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -888,24 +897,24 @@
         <v>16</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="2">
         <v>2</v>
@@ -913,12 +922,12 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2">
         <v>2</v>
@@ -928,7 +937,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D9" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F9" s="2">
         <v>2</v>
@@ -938,7 +947,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="2">
         <v>7</v>
@@ -948,7 +957,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="2">
         <v>7</v>
@@ -958,7 +967,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="2">
         <v>7</v>
@@ -968,7 +977,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="2">
         <v>7</v>
@@ -1007,31 +1016,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92676871-D33F-40B2-BC52-965592F8E2D5}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.08984375" customWidth="1"/>
-    <col min="2" max="3" width="14.81640625" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.81640625" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>1</v>
@@ -1040,27 +1049,30 @@
         <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1068,31 +1080,34 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>10</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>12</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D8" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>20</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -1100,24 +1115,30 @@
       <c r="H8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="I8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9">
         <v>4</v>
       </c>
       <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
         <v>19</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>7</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>10</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>4</v>
       </c>
     </row>
@@ -1131,7 +1152,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A7" sqref="A7:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1153,12 +1174,12 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -1182,12 +1203,12 @@
         <v>16</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -1196,7 +1217,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
@@ -1213,7 +1234,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1237,7 +1258,7 @@
         <v>25</v>
       </c>
       <c r="I8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1305,7 +1326,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1323,7 +1344,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -1347,12 +1368,12 @@
         <v>16</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -1361,7 +1382,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
@@ -1374,7 +1395,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1383,10 +1404,10 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F8" s="2">
         <v>4</v>
@@ -1394,7 +1415,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1405,13 +1426,13 @@
         <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1471,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10980A8C-B9E6-4B27-9B36-E6C7ECA340A8}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1496,12 +1517,12 @@
     </row>
     <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>1</v>
@@ -1525,12 +1546,12 @@
         <v>16</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>40</v>
+      <c r="A7" t="s">
+        <v>99</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>7</v>
@@ -1539,268 +1560,273 @@
         <v>12</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F7" s="7">
         <v>2</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D8" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F8" s="7">
         <v>2</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D9" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F9" s="7">
         <v>1.5</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D10" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F10" s="7">
         <v>3.5</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D11" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F11" s="7">
         <v>4</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D12" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F12" s="7">
         <v>1</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D13" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F13" s="7">
         <v>1.5</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D14" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F14" s="7">
         <v>2</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D15" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F15" s="7">
         <v>1.5</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D16" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F16" s="7">
         <v>3.5</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D17" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F17" s="7">
         <v>4</v>
       </c>
       <c r="I17" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D18" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D18" s="7" t="s">
-        <v>78</v>
-      </c>
       <c r="E18" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F18" s="7">
         <v>1</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D19" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F19" s="7">
         <v>1.5</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D20" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F20" s="7">
         <v>2</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D21" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F21" s="7">
         <v>1.5</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D22" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F22" s="7">
         <v>3.5</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D23" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F23" s="7">
         <v>4</v>
       </c>
       <c r="I23" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D24" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D24" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="F24" s="7">
         <v>1</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D25" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F25" s="7">
         <v>1.5</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1812,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3A90A2B-4A87-4E22-B487-EB4C75A41F7C}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1833,7 +1859,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>1</v>
@@ -1857,12 +1883,12 @@
         <v>16</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -1871,10 +1897,10 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F7" s="2">
         <v>8</v>
@@ -1886,7 +1912,7 @@
         <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1897,10 +1923,10 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F8" s="2">
         <f>0.5*64*3</f>
@@ -1914,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1925,10 +1951,10 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" t="s">
         <v>88</v>
-      </c>
-      <c r="E9" t="s">
-        <v>91</v>
       </c>
       <c r="F9" s="2">
         <f>64*3-F8</f>
@@ -1942,7 +1968,7 @@
         <v>192</v>
       </c>
       <c r="I9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1992,14 +2018,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B7DAB6-DEED-45AB-9771-D3A66CEC2077}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="17.08984375" customWidth="1"/>
     <col min="2" max="2" width="17.1796875" customWidth="1"/>
     <col min="3" max="3" width="14.453125" customWidth="1"/>
     <col min="4" max="4" width="16.90625" customWidth="1"/>
@@ -2013,7 +2040,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -2037,12 +2064,12 @@
         <v>16</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2051,18 +2078,23 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2072,10 +2104,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F6F36D-A4ED-4413-AD88-E672D69AFDF3}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2088,17 +2120,17 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -2122,21 +2154,26 @@
         <v>16</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2149,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F58817-5DC2-4070-BA26-CEF6806ABD5E}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2169,12 +2206,12 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -2198,12 +2235,12 @@
         <v>16</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2212,213 +2249,298 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F8" s="2">
         <v>2</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D10" t="s">
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F14" s="2">
         <v>1</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F17" s="2">
         <v>3</v>
       </c>
+      <c r="G17" s="2">
+        <v>3</v>
+      </c>
+      <c r="H17" s="2">
+        <v>3</v>
+      </c>
       <c r="I17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F18" s="2">
         <v>3</v>
       </c>
+      <c r="G18" s="2">
+        <v>3</v>
+      </c>
+      <c r="H18" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F19" s="2">
         <v>3</v>
       </c>
+      <c r="G19" s="2">
+        <v>3</v>
+      </c>
+      <c r="H19" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F20" s="2">
         <v>2</v>
       </c>
+      <c r="G20" s="2">
+        <v>2</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F21" s="2">
         <v>3</v>
       </c>
+      <c r="G21" s="2">
+        <v>3</v>
+      </c>
+      <c r="H21" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D22" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E22" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F22" s="2">
         <v>3</v>
       </c>
+      <c r="G22" s="2">
+        <v>3</v>
+      </c>
+      <c r="H22" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F23" s="2">
         <v>1</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1</v>
+      </c>
       <c r="I23" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
add carbon credit calcs
</commit_message>
<xml_diff>
--- a/R/data_raw/lca-sheets/enterprise-flows-all-areas.xlsx
+++ b/R/data_raw/lca-sheets/enterprise-flows-all-areas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\alfalfa\R\data_raw\lca-sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806B6B27-6E7B-4A00-AEE1-A72AC588716B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0275D51-BFB1-4CA8-A10F-C88891CB2947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="8" xr2:uid="{6B1DF06E-0D8B-4B6A-BB9B-61BA1D32BA21}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="7" activeTab="7" xr2:uid="{6B1DF06E-0D8B-4B6A-BB9B-61BA1D32BA21}"/>
   </bookViews>
   <sheets>
     <sheet name="meta-data" sheetId="10" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="fertility" sheetId="3" r:id="rId4"/>
     <sheet name="pesticide" sheetId="4" r:id="rId5"/>
     <sheet name="irrigation" sheetId="5" r:id="rId6"/>
-    <sheet name="soil_emissions" sheetId="6" r:id="rId7"/>
-    <sheet name="soil_c" sheetId="11" r:id="rId8"/>
+    <sheet name="soil_n2o" sheetId="6" r:id="rId7"/>
+    <sheet name="carbon_credits" sheetId="11" r:id="rId8"/>
     <sheet name="field_ops" sheetId="7" r:id="rId9"/>
     <sheet name="harvest_ops" sheetId="9" r:id="rId10"/>
   </sheets>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="106">
   <si>
     <t>units</t>
   </si>
@@ -176,18 +176,9 @@
     <t>3 year stand life</t>
   </si>
   <si>
-    <t>soil c</t>
-  </si>
-  <si>
-    <t>output??</t>
-  </si>
-  <si>
     <t>Taken from California healthy soils</t>
   </si>
   <si>
-    <t xml:space="preserve">Assumed the addition of a perennial crop in a basic cropping system </t>
-  </si>
-  <si>
     <t>This is the value used in the enterprise budget, or it represents the most 'representative' value</t>
   </si>
   <si>
@@ -363,6 +354,15 @@
   </si>
   <si>
     <t>disk border ridges</t>
+  </si>
+  <si>
+    <t>http://comet-planner-cdfahsp.com/</t>
+  </si>
+  <si>
+    <t>carbon_credit</t>
+  </si>
+  <si>
+    <t>n2o</t>
   </si>
 </sst>
 </file>
@@ -787,7 +787,7 @@
     </row>
     <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -798,21 +798,21 @@
     </row>
     <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -820,7 +820,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
@@ -828,7 +828,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -836,7 +836,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -922,7 +922,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -937,7 +937,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D9" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F9" s="2">
         <v>2</v>
@@ -1049,7 +1049,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>2</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -1217,7 +1217,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1258,7 +1258,7 @@
         <v>25</v>
       </c>
       <c r="I8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1373,7 +1373,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -1382,7 +1382,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1404,10 +1404,10 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F8" s="2">
         <v>4</v>
@@ -1415,7 +1415,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1426,13 +1426,13 @@
         <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1517,7 +1517,7 @@
     </row>
     <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1551,7 +1551,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>7</v>
@@ -1560,273 +1560,273 @@
         <v>12</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F7" s="7">
         <v>2</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D8" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F8" s="7">
         <v>2</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D9" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F9" s="7">
         <v>1.5</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D10" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F10" s="7">
         <v>3.5</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D11" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F11" s="7">
         <v>4</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D12" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F12" s="7">
         <v>1</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D13" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F13" s="7">
         <v>1.5</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D14" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F14" s="7">
         <v>2</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D15" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F15" s="7">
         <v>1.5</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D16" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F16" s="7">
         <v>3.5</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D17" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F17" s="7">
         <v>4</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D18" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F18" s="7">
         <v>1</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D19" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F19" s="7">
         <v>1.5</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D20" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F20" s="7">
         <v>2</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D21" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F21" s="7">
         <v>1.5</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D22" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F22" s="7">
         <v>3.5</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D23" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F23" s="7">
         <v>4</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D24" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F24" s="7">
         <v>1</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D25" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F25" s="7">
         <v>1.5</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -1900,7 +1900,7 @@
         <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F7" s="2">
         <v>8</v>
@@ -1912,7 +1912,7 @@
         <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1923,10 +1923,10 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F8" s="2">
         <f>0.5*64*3</f>
@@ -1940,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1951,10 +1951,10 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" t="s">
         <v>85</v>
-      </c>
-      <c r="E9" t="s">
-        <v>88</v>
       </c>
       <c r="F9" s="2">
         <f>64*3-F8</f>
@@ -1968,7 +1968,7 @@
         <v>192</v>
       </c>
       <c r="I9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -2069,7 +2069,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2078,23 +2078,23 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2104,10 +2104,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F6F36D-A4ED-4413-AD88-E672D69AFDF3}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2116,16 +2116,17 @@
     <col min="2" max="2" width="17.1796875" customWidth="1"/>
     <col min="3" max="3" width="14.453125" customWidth="1"/>
     <col min="4" max="4" width="16.90625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -2159,13 +2160,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -2173,7 +2174,44 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>96</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2186,7 +2224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F58817-5DC2-4070-BA26-CEF6806ABD5E}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2206,7 +2244,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -2240,7 +2278,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2249,10 +2287,10 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
@@ -2264,15 +2302,15 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F8" s="2">
         <v>2</v>
@@ -2289,7 +2327,7 @@
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
@@ -2306,7 +2344,7 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -2320,10 +2358,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -2337,10 +2375,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
@@ -2354,10 +2392,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
@@ -2371,10 +2409,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F14" s="2">
         <v>1</v>
@@ -2388,10 +2426,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
@@ -2405,10 +2443,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
@@ -2422,10 +2460,10 @@
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F17" s="2">
         <v>3</v>
@@ -2437,15 +2475,15 @@
         <v>3</v>
       </c>
       <c r="I17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F18" s="2">
         <v>3</v>
@@ -2459,10 +2497,10 @@
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F19" s="2">
         <v>3</v>
@@ -2476,10 +2514,10 @@
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F20" s="2">
         <v>2</v>
@@ -2493,10 +2531,10 @@
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F21" s="2">
         <v>3</v>
@@ -2510,10 +2548,10 @@
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F22" s="2">
         <v>3</v>
@@ -2527,10 +2565,10 @@
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F23" s="2">
         <v>1</v>

</xml_diff>